<commit_message>
update 14-04-2023 user reg verificatn done
</commit_message>
<xml_diff>
--- a/src/TestData.xlsx
+++ b/src/TestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13365" windowHeight="2790"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13365" windowHeight="3240"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Add_User" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:I5"/>
+  <oleSize ref="D1:I9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Email</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Full_Name</t>
   </si>
   <si>
-    <t>Erin Hermann</t>
-  </si>
-  <si>
     <t>DmItw6Ps!2</t>
   </si>
   <si>
@@ -63,19 +60,55 @@
     <t>Patrner_Password_Record</t>
   </si>
   <si>
-    <t>digitalmesh8hhwxd@maildrop.cc</t>
-  </si>
-  <si>
-    <t>DmBEMWPs!2</t>
-  </si>
-  <si>
-    <t>Sydni Anderson</t>
-  </si>
-  <si>
     <t>User_Password_Record</t>
   </si>
   <si>
-    <t>Dmhq64Ps!2</t>
+    <t>Email_ID</t>
+  </si>
+  <si>
+    <t>DmTs53Ps!2</t>
+  </si>
+  <si>
+    <t>User_Password</t>
+  </si>
+  <si>
+    <t>Irwin Hickle</t>
+  </si>
+  <si>
+    <t>digitalmeshp830DK@maildrop.cc</t>
+  </si>
+  <si>
+    <t>DmS2vSPs!2</t>
+  </si>
+  <si>
+    <t>Company_Name</t>
+  </si>
+  <si>
+    <t>digitalmeshp1fayy@maildrop.cc</t>
+  </si>
+  <si>
+    <t>eYYlB</t>
+  </si>
+  <si>
+    <t>DmcLYZPs!2</t>
+  </si>
+  <si>
+    <t>digitalmeshjjyfzh@maildrop.cc</t>
+  </si>
+  <si>
+    <t>idAsI</t>
+  </si>
+  <si>
+    <t>DmpKxvPs!2</t>
+  </si>
+  <si>
+    <t>digitalmesh5rb2yq@maildrop.cc</t>
+  </si>
+  <si>
+    <t>AaAch</t>
+  </si>
+  <si>
+    <t>DmQYmAPs!2</t>
   </si>
 </sst>
 </file>
@@ -408,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -422,11 +455,13 @@
     <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.58984375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.80859375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.91015625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -440,27 +475,30 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
-        <v>18</v>
+      <c r="J1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -469,19 +507,22 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
-        <v>19</v>
+      <c r="J2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -491,25 +532,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.390625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last update 14-04-2023 eve verfictn complete
</commit_message>
<xml_diff>
--- a/src/TestData.xlsx
+++ b/src/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13365" windowHeight="3240"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13365" windowHeight="3165"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Email</t>
   </si>
@@ -84,31 +84,31 @@
     <t>Company_Name</t>
   </si>
   <si>
-    <t>digitalmeshp1fayy@maildrop.cc</t>
-  </si>
-  <si>
-    <t>eYYlB</t>
-  </si>
-  <si>
-    <t>DmcLYZPs!2</t>
-  </si>
-  <si>
-    <t>digitalmeshjjyfzh@maildrop.cc</t>
-  </si>
-  <si>
-    <t>idAsI</t>
-  </si>
-  <si>
-    <t>DmpKxvPs!2</t>
-  </si>
-  <si>
-    <t>digitalmesh5rb2yq@maildrop.cc</t>
-  </si>
-  <si>
-    <t>AaAch</t>
-  </si>
-  <si>
-    <t>DmQYmAPs!2</t>
+    <t>PhoneNmbr</t>
+  </si>
+  <si>
+    <t>digitalmeshobxchz@maildrop.cc</t>
+  </si>
+  <si>
+    <t>4140662324</t>
+  </si>
+  <si>
+    <t>rcXvq</t>
+  </si>
+  <si>
+    <t>DmU31CPs!2</t>
+  </si>
+  <si>
+    <t>digitalmeshlj7ux5@maildrop.cc</t>
+  </si>
+  <si>
+    <t>3470414515</t>
+  </si>
+  <si>
+    <t>KyPsR</t>
+  </si>
+  <si>
+    <t>DmHsC3Ps!2</t>
   </si>
 </sst>
 </file>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -455,13 +455,14 @@
     <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.58984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0703125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="24.80859375" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="15.91015625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.1875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -492,8 +493,11 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -513,7 +517,7 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -523,6 +527,9 @@
       </c>
       <c r="J2" t="s">
         <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest update 19-04-2023 eve
</commit_message>
<xml_diff>
--- a/src/TestData.xlsx
+++ b/src/TestData.xlsx
@@ -12,12 +12,12 @@
     <sheet name="Add_Products" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:M11"/>
+  <oleSize ref="J1:N11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>Email</t>
   </si>
@@ -79,27 +79,9 @@
     <t>PhoneNmbr</t>
   </si>
   <si>
-    <t>Chaya Rosenbaum</t>
-  </si>
-  <si>
-    <t>digitalmeshJmRpZK@maildrop.cc</t>
-  </si>
-  <si>
     <t>Dm53mYDm1zNYPs!2</t>
   </si>
   <si>
-    <t>digitalmeshboexd4@maildrop.cc</t>
-  </si>
-  <si>
-    <t>2093647839</t>
-  </si>
-  <si>
-    <t>BgyvV</t>
-  </si>
-  <si>
-    <t>Dmxln3Ps!2</t>
-  </si>
-  <si>
     <t>Product_Name</t>
   </si>
   <si>
@@ -212,12 +194,55 @@
   </si>
   <si>
     <t>Free Delivery</t>
+  </si>
+  <si>
+    <t>Prod_Category_input</t>
+  </si>
+  <si>
+    <t>deodorisers</t>
+  </si>
+  <si>
+    <t>EcomcFbw</t>
+  </si>
+  <si>
+    <t>Product_Identifier_Value</t>
+  </si>
+  <si>
+    <t>Demarco Purdy II</t>
+  </si>
+  <si>
+    <t>digitalmeshRtUaWD@maildrop.cc</t>
+  </si>
+  <si>
+    <t>digitalmeshangeb7@maildrop.cc</t>
+  </si>
+  <si>
+    <t>2622922229</t>
+  </si>
+  <si>
+    <t>UGCVF</t>
+  </si>
+  <si>
+    <t>DmBzMHPs!2</t>
+  </si>
+  <si>
+    <t>EcomepH3</t>
+  </si>
+  <si>
+    <t>ProdIdBI5b</t>
+  </si>
+  <si>
+    <t>EcomyyyG</t>
+  </si>
+  <si>
+    <t>ProdIdGcPx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -264,10 +289,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -566,22 +593,22 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -639,19 +666,19 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -669,9 +696,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -687,13 +714,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -703,199 +730,249 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" customWidth="1"/>
-    <col min="14" max="14" width="31.42578125" customWidth="1"/>
-    <col min="15" max="15" width="21" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" customWidth="1"/>
-    <col min="17" max="17" width="25.28515625" customWidth="1"/>
-    <col min="18" max="18" width="29" customWidth="1"/>
-    <col min="19" max="19" width="26.42578125" customWidth="1"/>
-    <col min="20" max="20" width="28.28515625" customWidth="1"/>
-    <col min="21" max="21" width="21.28515625" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" customWidth="1"/>
-    <col min="23" max="23" width="19.42578125" customWidth="1"/>
-    <col min="24" max="24" width="60.5703125" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2500</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3500</v>
+      </c>
+      <c r="H2" s="3">
+        <v>3600</v>
+      </c>
+      <c r="I2" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J2" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="L2" s="3">
+        <v>20</v>
+      </c>
+      <c r="M2" s="3">
+        <v>25</v>
+      </c>
+      <c r="N2" s="3">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="3">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="3">
+        <v>20</v>
+      </c>
+      <c r="S2" s="3">
+        <v>20</v>
+      </c>
+      <c r="T2" s="3">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="3">
+        <v>50</v>
+      </c>
+      <c r="W2" t="s">
         <v>54</v>
       </c>
-      <c r="S1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="X2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="U1" t="s">
-        <v>57</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="Y2" t="s">
         <v>58</v>
       </c>
-      <c r="W1" t="s">
-        <v>59</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Z2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" t="s">
-        <v>63</v>
+      <c r="AB2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2">
-        <v>2500</v>
-      </c>
-      <c r="G2">
-        <v>350000</v>
-      </c>
-      <c r="H2">
-        <v>30000</v>
-      </c>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2">
-        <v>20</v>
-      </c>
-      <c r="M2">
-        <v>25</v>
-      </c>
-      <c r="N2">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2">
-        <v>20</v>
-      </c>
-      <c r="S2">
-        <v>20</v>
-      </c>
-      <c r="T2">
-        <v>20</v>
-      </c>
-      <c r="U2" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2">
-        <v>50</v>
-      </c>
-      <c r="W2" t="s">
-        <v>60</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>64</v>
-      </c>
+    <row r="3" spans="1:29">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
     </row>
-    <row r="3" spans="1:25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
+    <row r="4" spans="1:29">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Latest update 19-04-2023 eveng last
</commit_message>
<xml_diff>
--- a/src/TestData.xlsx
+++ b/src/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
   <si>
     <t>Email</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>ProdIdGcPx</t>
+  </si>
+  <si>
+    <t>EcomvMFj</t>
+  </si>
+  <si>
+    <t>ProdId0Svp</t>
   </si>
 </sst>
 </file>
@@ -730,7 +736,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -860,6 +866,9 @@
       <c r="AD1" t="s">
         <v>28</v>
       </c>
+      <c r="AE1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" t="s">
@@ -944,13 +953,16 @@
         <v>61</v>
       </c>
       <c r="AB2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AC2" t="s">
         <v>69</v>
       </c>
       <c r="AD2" t="s">
         <v>71</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:29">

</xml_diff>